<commit_message>
added milestone 2 tasks
</commit_message>
<xml_diff>
--- a/Lhub_Sch.xlsx
+++ b/Lhub_Sch.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farah\Desktop\V1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Project management\Learning-hub project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Task ID</t>
   </si>
@@ -40,36 +40,6 @@
   </si>
   <si>
     <t>https://www.vertex42.com/Files/download2/gdrive.php?file=project-schedule</t>
-  </si>
-  <si>
-    <t>Lhub_PP_V1</t>
-  </si>
-  <si>
-    <t>Lhub_Sch_V1</t>
-  </si>
-  <si>
-    <t>Lhub_CMP_V1</t>
-  </si>
-  <si>
-    <t>Lhub_RSK_V1</t>
-  </si>
-  <si>
-    <t>Lhub_RTM_V1</t>
-  </si>
-  <si>
-    <t>Lhub_SIQ_V1</t>
-  </si>
-  <si>
-    <t>Lhub_PR_V1</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_V1</t>
-  </si>
-  <si>
-    <t>Lhub_PT_V1</t>
-  </si>
-  <si>
-    <t>Lhub_RSK_V1, Lhub_Sch_V1 , Lhub_Issue_V1, Lhub_PT_V1 , Lhub_SIQ_V1 , Lhub_CMP_V1</t>
   </si>
   <si>
     <r>
@@ -137,7 +107,49 @@
     <t xml:space="preserve">Status </t>
   </si>
   <si>
-    <t>Lhub_ISSUE_V1</t>
+    <t>Lhub_PP</t>
+  </si>
+  <si>
+    <t>Lhub_Sch</t>
+  </si>
+  <si>
+    <t>Lhub_CMP</t>
+  </si>
+  <si>
+    <t>Lhub_RSK</t>
+  </si>
+  <si>
+    <t>Lhub_Issue</t>
+  </si>
+  <si>
+    <t>Lhub_SRS</t>
+  </si>
+  <si>
+    <t>Lhub_RTM</t>
+  </si>
+  <si>
+    <t>Lhub_SIQ</t>
+  </si>
+  <si>
+    <t>Lhub_PR</t>
+  </si>
+  <si>
+    <t>Lhub_PT</t>
+  </si>
+  <si>
+    <t>Lhub_RSK, Lhub_Sch , Lhub_Issue, Lhub_PT , Lhub_SIQ , Lhub_CMP</t>
+  </si>
+  <si>
+    <t>Lhub_SDD</t>
+  </si>
+  <si>
+    <t>Software design document (SDD)</t>
+  </si>
+  <si>
+    <t>Lhub_DesignPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">design peer review sheet </t>
   </si>
 </sst>
 </file>
@@ -343,9 +355,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -358,9 +368,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -373,16 +381,14 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -420,18 +426,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -446,6 +440,30 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,10 +773,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -773,7 +791,7 @@
     <col min="8" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="19" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="15" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -781,47 +799,47 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
     </row>
     <row r="2" spans="1:27" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>7</v>
+      <c r="A2" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C2" s="8">
         <v>3</v>
@@ -830,19 +848,19 @@
         <v>2</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="12" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
-        <v>8</v>
+      <c r="A3" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C3" s="8">
         <v>2</v>
@@ -853,15 +871,15 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="12" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
-        <v>9</v>
+      <c r="A4" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C4" s="8">
         <v>3</v>
@@ -874,12 +892,12 @@
         <v>3</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
-        <v>10</v>
+      <c r="A5" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>4</v>
@@ -891,16 +909,16 @@
         <v>2</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" ht="39" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
-        <v>30</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>5</v>
@@ -912,19 +930,19 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="12" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="C7" s="8">
         <v>4</v>
@@ -935,15 +953,15 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="12" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>11</v>
+      <c r="A8" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C8" s="9">
         <v>2</v>
@@ -952,19 +970,19 @@
         <v>1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="12" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
-        <v>12</v>
+      <c r="A9" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C9" s="9">
         <v>1</v>
@@ -973,19 +991,19 @@
         <v>3</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="12" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="39" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
-        <v>13</v>
+      <c r="A10" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C10" s="9">
         <v>2</v>
@@ -994,43 +1012,73 @@
         <v>3</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" ht="39.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="39" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="20">
         <v>2</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="20">
         <v>1</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="15" t="s">
+      <c r="E11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="G11" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" s="25" customFormat="1" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2</v>
+      </c>
+      <c r="D12" s="8">
+        <v>3</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" s="25" customFormat="1" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E14" s="2"/>
@@ -1041,96 +1089,96 @@
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-    </row>
-    <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="5"/>
+    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+    </row>
+    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="5"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
@@ -5006,18 +5054,26 @@
       <c r="E1000" s="2"/>
       <c r="F1000" s="2"/>
     </row>
+    <row r="1001" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E1001" s="2"/>
+      <c r="F1001" s="2"/>
+    </row>
+    <row r="1002" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E1002" s="2"/>
+      <c r="F1002" s="2"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1000">
+  <conditionalFormatting sqref="G1:G1002">
     <cfRule type="beginsWith" dxfId="2" priority="1" operator="beginsWith" text="done">
       <formula>LEFT((G1),LEN("done"))=("done")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1000">
+  <conditionalFormatting sqref="G1:G1002">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="in progress">
       <formula>NOT(ISERROR(SEARCH(("in progress"),(G1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1000">
+  <conditionalFormatting sqref="G1:G1002">
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="not done">
       <formula>NOT(ISERROR(SEARCH(("not done"),(G1))))</formula>
     </cfRule>

</xml_diff>